<commit_message>
qpp018 merge personal and company report
</commit_message>
<xml_diff>
--- a/nts.uk/file/pr/nts.uk.file.pr.infra/src/main/resources/report/SocialInsuMergeLayoutTemplate.xlsx
+++ b/nts.uk/file/pr/nts.uk.file.pr.infra/src/main/resources/report/SocialInsuMergeLayoutTemplate.xlsx
@@ -422,6 +422,30 @@
     <xf numFmtId="37" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="37" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -451,30 +475,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -799,7 +799,7 @@
   <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScale="110" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="A4" sqref="A4:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -813,132 +813,132 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" s="45"/>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="45"/>
-      <c r="M2" s="45"/>
-      <c r="N2" s="45"/>
-      <c r="O2" s="45"/>
+      <c r="A2" s="30"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5" s="44" t="s">
+      <c r="A5" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="44"/>
-      <c r="C5" s="44"/>
-      <c r="D5" s="44"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A6" s="44" t="s">
+      <c r="A6" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="44"/>
-      <c r="C6" s="44"/>
-      <c r="D6" s="44"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
     </row>
     <row r="7" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="43" t="s">
+      <c r="A7" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="43"/>
-      <c r="C7" s="40" t="s">
+      <c r="B7" s="32"/>
+      <c r="C7" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="40" t="s">
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="H7" s="41"/>
-      <c r="I7" s="41"/>
-      <c r="J7" s="42"/>
-      <c r="K7" s="40" t="s">
+      <c r="H7" s="34"/>
+      <c r="I7" s="34"/>
+      <c r="J7" s="35"/>
+      <c r="K7" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="L7" s="41"/>
-      <c r="M7" s="41"/>
-      <c r="N7" s="42"/>
-      <c r="O7" s="39" t="s">
+      <c r="L7" s="34"/>
+      <c r="M7" s="34"/>
+      <c r="N7" s="35"/>
+      <c r="O7" s="36" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="43"/>
-      <c r="B8" s="43"/>
-      <c r="C8" s="40" t="s">
+      <c r="A8" s="32"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="41"/>
-      <c r="E8" s="40" t="s">
+      <c r="D8" s="34"/>
+      <c r="E8" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="41"/>
-      <c r="G8" s="40" t="s">
+      <c r="F8" s="34"/>
+      <c r="G8" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="H8" s="41"/>
-      <c r="I8" s="40" t="s">
+      <c r="H8" s="34"/>
+      <c r="I8" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="J8" s="41"/>
-      <c r="K8" s="40" t="s">
+      <c r="J8" s="34"/>
+      <c r="K8" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="L8" s="41"/>
-      <c r="M8" s="40" t="s">
+      <c r="L8" s="34"/>
+      <c r="M8" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="N8" s="41"/>
-      <c r="O8" s="39"/>
+      <c r="N8" s="34"/>
+      <c r="O8" s="36"/>
     </row>
     <row r="9" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="43"/>
-      <c r="B9" s="43"/>
+      <c r="A9" s="32"/>
+      <c r="B9" s="32"/>
       <c r="C9" s="6" t="s">
         <v>11</v>
       </c>
@@ -975,7 +975,7 @@
       <c r="N9" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="O9" s="39"/>
+      <c r="O9" s="36"/>
     </row>
     <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="7"/>
@@ -1012,30 +1012,30 @@
       <c r="O11" s="21"/>
     </row>
     <row r="12" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="33" t="s">
+      <c r="A12" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="34"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="30"/>
+      <c r="B12" s="42"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="38"/>
       <c r="E12" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="33" t="s">
+      <c r="F12" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="G12" s="34"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="36"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="43"/>
+      <c r="I12" s="44"/>
       <c r="J12" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="K12" s="37" t="s">
+      <c r="K12" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="L12" s="38"/>
-      <c r="M12" s="29"/>
-      <c r="N12" s="30"/>
+      <c r="L12" s="46"/>
+      <c r="M12" s="37"/>
+      <c r="N12" s="38"/>
     </row>
     <row r="13" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="2"/>
@@ -1044,12 +1044,12 @@
       <c r="H13" s="13"/>
       <c r="I13" s="13"/>
       <c r="J13" s="13"/>
-      <c r="K13" s="31" t="s">
+      <c r="K13" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="L13" s="31"/>
-      <c r="M13" s="32"/>
-      <c r="N13" s="32"/>
+      <c r="L13" s="39"/>
+      <c r="M13" s="40"/>
+      <c r="N13" s="40"/>
     </row>
     <row r="14" spans="1:15" s="1" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="22"/>
@@ -1093,22 +1093,6 @@
     <row r="21" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="A1:O2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="A7:B9"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G7:J7"/>
-    <mergeCell ref="O7:O9"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="K7:N7"/>
     <mergeCell ref="M12:N12"/>
     <mergeCell ref="K13:L13"/>
     <mergeCell ref="M13:N13"/>
@@ -1117,14 +1101,27 @@
     <mergeCell ref="F12:G12"/>
     <mergeCell ref="H12:I12"/>
     <mergeCell ref="K12:L12"/>
+    <mergeCell ref="O7:O9"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="K7:N7"/>
+    <mergeCell ref="A7:B9"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G7:J7"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A1:O2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A5:D5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="55" orientation="landscape" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <headerFooter>
-    <oddHeader>&amp;L 【日通 システム株式会社】</oddHeader>
-  </headerFooter>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="1" OnePage="0" WScale="100"/>

</xml_diff>